<commit_message>
new_test integrated skill from different experiences added
</commit_message>
<xml_diff>
--- a/upload_files/CV2_1__text.xlsx
+++ b/upload_files/CV2_1__text.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="171">
   <si>
     <t>CV ID</t>
   </si>
@@ -55,16 +55,16 @@
     <t>text.txt</t>
   </si>
   <si>
-    <t>37.62</t>
-  </si>
-  <si>
-    <t>oracle dba : 1</t>
-  </si>
-  <si>
-    <t>dba : 8</t>
-  </si>
-  <si>
-    <t>oracle database : 26</t>
+    <t>27.81</t>
+  </si>
+  <si>
+    <t>oracle dba : 2</t>
+  </si>
+  <si>
+    <t>dba : 7</t>
+  </si>
+  <si>
+    <t>oracle database : 28</t>
   </si>
   <si>
     <t>database administrator : 7</t>
@@ -73,22 +73,16 @@
     <t>administrator : 7</t>
   </si>
   <si>
-    <t>coding : 1</t>
-  </si>
-  <si>
-    <t>testing : 3</t>
+    <t>testing : 2</t>
   </si>
   <si>
     <t>database : 35</t>
   </si>
   <si>
-    <t>oracle : 33</t>
-  </si>
-  <si>
-    <t>communication : 2</t>
-  </si>
-  <si>
-    <t>interpersonal skills : 3</t>
+    <t>oracle : 32</t>
+  </si>
+  <si>
+    <t>interpersonal skills : 4</t>
   </si>
   <si>
     <t>analytical : 1</t>
@@ -106,7 +100,7 @@
     <t>ms sql : 2</t>
   </si>
   <si>
-    <t>sql server : 3</t>
+    <t>sql server : 4</t>
   </si>
   <si>
     <t>jdbc : 2</t>
@@ -127,13 +121,13 @@
     <t>toad : 2</t>
   </si>
   <si>
-    <t>rman : 11</t>
+    <t>rman : 14</t>
   </si>
   <si>
     <t>asm : 3</t>
   </si>
   <si>
-    <t>oem : 4</t>
+    <t>oem : 5</t>
   </si>
   <si>
     <t>grid : 6</t>
@@ -148,10 +142,10 @@
     <t>emc : 2</t>
   </si>
   <si>
-    <t>dynatrace : 3</t>
-  </si>
-  <si>
-    <t>mysql : 4</t>
+    <t>dynatrace : 5</t>
+  </si>
+  <si>
+    <t>mysql : 5</t>
   </si>
   <si>
     <t>encryption : 1</t>
@@ -163,10 +157,7 @@
     <t>solaris : 3</t>
   </si>
   <si>
-    <t>windows : 3</t>
-  </si>
-  <si>
-    <t>unix : 4</t>
+    <t>unix : 3</t>
   </si>
   <si>
     <t>linux : 4</t>
@@ -175,7 +166,7 @@
     <t>database administration : 6</t>
   </si>
   <si>
-    <t>administration : 19</t>
+    <t>administration : 20</t>
   </si>
   <si>
     <t>postgresql : 3</t>
@@ -187,40 +178,37 @@
     <t>weblogic : 2</t>
   </si>
   <si>
-    <t>performance tuning : 8</t>
-  </si>
-  <si>
-    <t>tuning : 9</t>
-  </si>
-  <si>
-    <t>monitoring : 10</t>
-  </si>
-  <si>
-    <t>backup : 7</t>
+    <t>performance tuning : 7</t>
+  </si>
+  <si>
+    <t>tuning : 11</t>
+  </si>
+  <si>
+    <t>monitoring : 12</t>
+  </si>
+  <si>
+    <t>backup : 8</t>
   </si>
   <si>
     <t>recovery : 9</t>
   </si>
   <si>
-    <t>shell scripting : 3</t>
+    <t>shell scripting : 4</t>
   </si>
   <si>
     <t>scripting : 2</t>
   </si>
   <si>
-    <t>maintenance : 12</t>
-  </si>
-  <si>
     <t>oracle rac : 1</t>
   </si>
   <si>
-    <t>rac : 3</t>
+    <t>rac : 4</t>
   </si>
   <si>
     <t>installation : 6</t>
   </si>
   <si>
-    <t>patching : 6</t>
+    <t>patching : 8</t>
   </si>
   <si>
     <t>migration : 6</t>
@@ -229,34 +217,31 @@
     <t>sql tuning : 1</t>
   </si>
   <si>
-    <t>production : 12</t>
+    <t>production : 11</t>
   </si>
   <si>
     <t>deployment : 1</t>
   </si>
   <si>
-    <t>code : 1</t>
-  </si>
-  <si>
     <t>reporting : 7</t>
   </si>
   <si>
-    <t>enterprise manager : 7</t>
+    <t>enterprise manager : 8</t>
   </si>
   <si>
     <t>manager : 7</t>
   </si>
   <si>
-    <t>performance monitoring : 4</t>
+    <t>performance monitoring : 6</t>
   </si>
   <si>
     <t>sql : 9</t>
   </si>
   <si>
-    <t>databases : 20</t>
-  </si>
-  <si>
-    <t>communication skills : 1</t>
+    <t>databases : 19</t>
+  </si>
+  <si>
+    <t>communication skills : 2</t>
   </si>
   <si>
     <t>design : 7</t>
@@ -268,13 +253,10 @@
     <t>customer service : 3</t>
   </si>
   <si>
-    <t>project : 9</t>
-  </si>
-  <si>
     <t>research : 1</t>
   </si>
   <si>
-    <t>configuration : 7</t>
+    <t>configuration : 8</t>
   </si>
   <si>
     <t>legal : 1</t>
@@ -283,10 +265,7 @@
     <t>security : 3</t>
   </si>
   <si>
-    <t>development : 9</t>
-  </si>
-  <si>
-    <t>troubleshooting : 3</t>
+    <t>troubleshooting : 4</t>
   </si>
   <si>
     <t>systems : 2</t>
@@ -301,13 +280,13 @@
     <t>red hat : 1</t>
   </si>
   <si>
-    <t>operating system : 3</t>
-  </si>
-  <si>
-    <t>scheduling : 5</t>
-  </si>
-  <si>
-    <t>capacity planning : 2</t>
+    <t>operating system : 2</t>
+  </si>
+  <si>
+    <t>scheduling : 4</t>
+  </si>
+  <si>
+    <t>capacity planning : 3</t>
   </si>
   <si>
     <t>planning : 4</t>
@@ -349,7 +328,7 @@
     <t>tibco : 1</t>
   </si>
   <si>
-    <t>shell scripts : 4</t>
+    <t>shell scripts : 3</t>
   </si>
   <si>
     <t>tables : 5</t>
@@ -370,7 +349,7 @@
     <t>production support : 2</t>
   </si>
   <si>
-    <t>requests : 1</t>
+    <t>requests : 2</t>
   </si>
   <si>
     <t>business requirements : 5</t>
@@ -409,13 +388,13 @@
     <t>programmer : 1</t>
   </si>
   <si>
-    <t>analyst : 2</t>
+    <t>analyst : 3</t>
   </si>
   <si>
     <t>information system : 1</t>
   </si>
   <si>
-    <t>stored procedures : 2</t>
+    <t>stored procedures : 1</t>
   </si>
   <si>
     <t>debugging : 1</t>
@@ -424,7 +403,7 @@
     <t>application development : 1</t>
   </si>
   <si>
-    <t>r&amp;d : 3</t>
+    <t>r&amp;d : 4</t>
   </si>
   <si>
     <t>pl : 5</t>
@@ -442,7 +421,7 @@
     <t>business process : 3</t>
   </si>
   <si>
-    <t>data warehouse : 3</t>
+    <t>data warehouse : 4</t>
   </si>
   <si>
     <t>warehouse : 7</t>
@@ -463,7 +442,7 @@
     <t>metadata : 1</t>
   </si>
   <si>
-    <t>data extraction : 2</t>
+    <t>data extraction : 1</t>
   </si>
   <si>
     <t>sql scripts : 2</t>
@@ -505,55 +484,46 @@
     <t>reports : 1</t>
   </si>
   <si>
-    <t>training : 8</t>
-  </si>
-  <si>
     <t>computer applications : 2</t>
   </si>
   <si>
     <t>computer science : 4</t>
   </si>
   <si>
+    <t>data protection : 1</t>
+  </si>
+  <si>
     <t>foundation : 1</t>
   </si>
   <si>
     <t>service management : 1</t>
   </si>
   <si>
-    <t>data protection : 1</t>
-  </si>
-  <si>
-    <t>oracle e-business suite : 1</t>
+    <t>oracle e-business suite : 2</t>
   </si>
   <si>
     <t>ms sql server : 1</t>
   </si>
   <si>
-    <t>pl/sql : 1</t>
-  </si>
-  <si>
-    <t>project : 1</t>
+    <t>unix shell scripts : 2</t>
+  </si>
+  <si>
+    <t>sql : 1</t>
   </si>
   <si>
     <t>analysis : 1</t>
   </si>
   <si>
-    <t>sql : 1</t>
-  </si>
-  <si>
     <t>databases : 2</t>
   </si>
   <si>
-    <t>38.88</t>
+    <t>28.57</t>
+  </si>
+  <si>
+    <t>requests : 3</t>
   </si>
   <si>
     <t>process : 1</t>
-  </si>
-  <si>
-    <t>requests : 3</t>
-  </si>
-  <si>
-    <t>30.0</t>
   </si>
   <si>
     <t>0.0</t>
@@ -897,7 +867,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K159"/>
+  <dimension ref="A1:K151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -965,19 +935,19 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>164</v>
       </c>
       <c r="G2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="H2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I2" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="K2" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -985,10 +955,10 @@
         <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="H3" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -996,10 +966,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
-      </c>
-      <c r="H4" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1007,32 +974,23 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="E6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="F7" t="s">
-        <v>175</v>
-      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="E9" t="s">
@@ -1747,46 +1705,6 @@
     <row r="151" spans="5:5">
       <c r="E151" t="s">
         <v>163</v>
-      </c>
-    </row>
-    <row r="152" spans="5:5">
-      <c r="E152" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="153" spans="5:5">
-      <c r="E153" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="154" spans="5:5">
-      <c r="E154" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="155" spans="5:5">
-      <c r="E155" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="156" spans="5:5">
-      <c r="E156" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="157" spans="5:5">
-      <c r="E157" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="158" spans="5:5">
-      <c r="E158" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="159" spans="5:5">
-      <c r="E159" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>